<commit_message>
Se termino de realizar la funcionalidad para crear Venta
</commit_message>
<xml_diff>
--- a/CapaPresentacionAdmin/Templates/Royal Tech - Historial_de_Ventas.xlsx
+++ b/CapaPresentacionAdmin/Templates/Royal Tech - Historial_de_Ventas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\CursoMVC\DiazDaniel-01\CursoMVC\CapaPresentacionAdmin\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173A47BD-3DF9-409F-BC03-E0E63F1D70C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A3E4C30-94E8-47A3-B45A-AAF92FC41B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5CEDC877-D8D9-4C14-95E6-DD58BA52BB65}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,18 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Av. Piedra Buena 3595</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>La Bondioleta</t>
   </si>
   <si>
     <t>1439 Mataderos (CABA)</t>
   </si>
   <si>
-    <t>011 4602-9300</t>
-  </si>
-  <si>
-    <t>La Bondioleta</t>
+    <t>+54 9 11 6766-7120</t>
+  </si>
+  <si>
+    <t>Reporte de Ventas</t>
   </si>
   <si>
     <t>Fecha de Inicio</t>
@@ -73,9 +75,6 @@
   </si>
   <si>
     <t>Id. Transaccion</t>
-  </si>
-  <si>
-    <t>Reporte de Ventas</t>
   </si>
 </sst>
 </file>
@@ -85,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$ $]#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,7 +134,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +147,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -241,56 +246,60 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -317,8 +326,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA0DC28-E10A-0928-A1FD-342983D50D36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5019675" y="276225"/>
+          <a:ext cx="1581150" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -614,267 +672,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D33FB2-712E-45F3-96E9-91251D9919C3}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="20" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="36" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="8"/>
+      <c r="B4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="8"/>
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.25" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="42.75" customHeight="1">
+      <c r="C8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="18"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="19"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="42.75" x14ac:dyDescent="0.6">
-      <c r="C9" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="11" t="s">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="45" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="10" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="30">
+      <c r="A13" s="3"/>
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="5.25" hidden="1" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>